<commit_message>
Added more physical constraints
</commit_message>
<xml_diff>
--- a/PiroverChassis_v5.0.xlsx
+++ b/PiroverChassis_v5.0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Pirover\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{182D2FE6-4F5E-4ED8-B146-40366D2157DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4343C5A-302E-47CA-9664-A9F2C149CD98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Terrain</t>
   </si>
@@ -36,9 +36,6 @@
     <t>Maximum Load (kg)</t>
   </si>
   <si>
-    <t>Locomotion Goals</t>
-  </si>
-  <si>
     <t>W</t>
   </si>
   <si>
@@ -48,9 +45,6 @@
     <t>H</t>
   </si>
   <si>
-    <t>Bounding Box (meters)</t>
-  </si>
-  <si>
     <t>Desired System Requirements</t>
   </si>
   <si>
@@ -58,6 +52,18 @@
   </si>
   <si>
     <t>Speed under Max Load(m/s)</t>
+  </si>
+  <si>
+    <t>Locomotion</t>
+  </si>
+  <si>
+    <t>Wheel Diameter (cm)</t>
+  </si>
+  <si>
+    <t>Component Sizes</t>
+  </si>
+  <si>
+    <t>Bounding Box (cm)</t>
   </si>
 </sst>
 </file>
@@ -381,10 +387,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -392,11 +398,12 @@
     <col min="1" max="1" width="28.7109375" customWidth="1"/>
     <col min="2" max="2" width="18.5703125" customWidth="1"/>
     <col min="3" max="3" width="28" customWidth="1"/>
+    <col min="7" max="7" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -404,21 +411,24 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
+      <c r="G2" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -426,21 +436,44 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>6</v>
-      </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>4.5</v>
+      </c>
+      <c r="C4">
+        <v>0.2</v>
+      </c>
+      <c r="D4">
+        <v>25</v>
+      </c>
+      <c r="E4">
+        <v>30</v>
+      </c>
+      <c r="F4">
+        <v>15</v>
+      </c>
+      <c r="G4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>